<commit_message>
REPORTGEN-706: Add option to not display source code in LIST_RULES_VIOLATIONS_BOOKMARKS
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2677FF3D-15CC-4742-BA36-1637661B4901}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E61094-E3B7-4391-AC5F-E7C695CEDF37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="701" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="253">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -934,9 +934,6 @@
       </rPr>
       <t>=true : add this one if you have specified a category in STD and want the evolution of the tags associated to this category (not specified by default)</t>
     </r>
-  </si>
-  <si>
-    <t>NEW</t>
   </si>
   <si>
     <t>* Block Name = QUALITY_TAGS_RULES_EVOLUTION</t>
@@ -1715,33 +1712,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="33"/>
       <c r="G1" s="33"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1749,7 +1746,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
       <c r="D3" s="3"/>
@@ -1757,7 +1754,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
       <c r="D4" s="3"/>
@@ -1765,54 +1762,54 @@
       <c r="F4" s="1"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="17"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="10" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>77</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="13" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="36"/>
       <c r="D20" s="36"/>
       <c r="E20" s="36"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
       <c r="E21" s="32"/>
@@ -1820,7 +1817,7 @@
       <c r="G21" s="34"/>
       <c r="H21" s="34"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="32"/>
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
@@ -1828,7 +1825,7 @@
       <c r="G22" s="34"/>
       <c r="H22" s="34"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
       <c r="F23" s="11"/>
     </row>
@@ -1857,57 +1854,59 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C1" s="30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23"/>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23"/>
     </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>185</v>
       </c>
@@ -1920,112 +1919,109 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A48014B-133C-4EB1-BCC8-C47F0FE2BA42}">
-  <dimension ref="B1:C20"/>
+  <dimension ref="B1:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="31" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="31" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -2042,51 +2038,51 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>202</v>
       </c>
@@ -2105,52 +2101,52 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>205</v>
       </c>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
     </row>
   </sheetData>
@@ -2167,86 +2163,86 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="24"/>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>227</v>
       </c>
@@ -2265,56 +2261,56 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
     </row>
   </sheetData>
@@ -2331,46 +2327,46 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23"/>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
     </row>
   </sheetData>
@@ -2387,54 +2383,54 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23"/>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>239</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2451,55 +2447,53 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
-    <col min="3" max="3" width="109.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C1" s="30"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="C1" s="30" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23"/>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23"/>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>244</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2515,643 +2509,643 @@
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="18" customWidth="1"/>
     <col min="6" max="7" width="38" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="18"/>
-    <col min="11" max="11" width="14.33203125" style="18" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" style="18" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="18"/>
+    <col min="8" max="8" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="18"/>
+    <col min="11" max="11" width="14.28515625" style="18" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="18" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B53" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B58" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B63" s="19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B73" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B78" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B83" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B88" s="19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B95" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B102" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B109" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B114" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B119" s="19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B124" s="19" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B129" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B134" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B143" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B144" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B145" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B146" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B147" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B148" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B149" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="18" t="s">
         <v>119</v>
       </c>
@@ -3170,19 +3164,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -3190,7 +3184,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -3198,7 +3192,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -3206,7 +3200,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -3224,32 +3218,32 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>60</v>
       </c>
@@ -3257,7 +3251,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>62</v>
       </c>
@@ -3265,7 +3259,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>64</v>
       </c>
@@ -3273,19 +3267,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3308,22 +3302,22 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>82</v>
       </c>
@@ -3331,7 +3325,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>83</v>
       </c>
@@ -3339,7 +3333,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>84</v>
       </c>
@@ -3347,7 +3341,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>85</v>
       </c>
@@ -3355,7 +3349,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>86</v>
       </c>
@@ -3363,7 +3357,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>87</v>
       </c>
@@ -3371,7 +3365,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>88</v>
       </c>
@@ -3379,7 +3373,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>89</v>
       </c>
@@ -3387,7 +3381,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>90</v>
       </c>
@@ -3395,7 +3389,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>102</v>
       </c>
@@ -3403,8 +3397,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>101</v>
       </c>
@@ -3422,92 +3416,92 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>146</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>164</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>150</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>148</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3526,47 +3520,47 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>171</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>153</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>154</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -19952,35 +19946,35 @@
       <c r="XFC6" s="22"/>
       <c r="XFD6" s="22"/>
     </row>
-    <row r="7" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>156</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -19999,62 +19993,62 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>160</v>
       </c>
@@ -20068,79 +20062,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
   <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="30" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>203</v>
       </c>
       <c r="C7" s="24"/>
     </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C8" s="24"/>
     </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23"/>
     </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>204</v>
       </c>

</xml_diff>

<commit_message>
REPORTGEN-705: Add rule description on option in component  RULES_LIST_STATISTICS_RATIO
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E61094-E3B7-4391-AC5F-E7C695CEDF37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6198D28-BF05-4E3D-BEC3-BC8B8A31A131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="253">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -656,9 +656,6 @@
   </si>
   <si>
     <t>RepGen:TABLE;RULES_LIST_LARGEST_VARIATION;BCID=60011,VARIATION=decrease,DATA=number,COUNT=50</t>
-  </si>
-  <si>
-    <t>*  LBL=violations or vulnerabilities (vulnerabilities if not set), this change the headers from Vulnerabilities to Violations</t>
   </si>
   <si>
     <t>RepGen:TABLE;RULES_LIST_STATISTICS_RATIO;METRICS=CISQ-Security,COMPLIANCE=true,LBL=violations</t>
@@ -985,6 +982,9 @@
   </si>
   <si>
     <t>* EVOLUTION=true|false. For display of added and removed columns. If not exists, the colums are displayed only if there is a previous snapshot</t>
+  </si>
+  <si>
+    <t>* DESC=true|false. For display rationale, description and remediation of the rule. By default if not present, it is false</t>
   </si>
 </sst>
 </file>
@@ -1712,7 +1712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1861,10 +1861,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1879,12 +1879,12 @@
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1968,22 +1968,22 @@
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -1996,7 +1996,7 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
@@ -2011,17 +2011,17 @@
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="31" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2109,13 +2109,13 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
@@ -2125,7 +2125,7 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2135,7 +2135,7 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2171,12 +2171,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2186,37 +2186,37 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2224,27 +2224,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2269,12 +2269,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2284,17 +2284,17 @@
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -2307,7 +2307,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2335,12 +2335,12 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
@@ -2363,7 +2363,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2390,23 +2390,23 @@
   <sheetData>
     <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2419,7 +2419,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2455,18 +2455,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C1" s="30"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2482,7 +2482,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2493,7 +2493,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -20060,10 +20060,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
-  <dimension ref="B1:C14"/>
+  <dimension ref="B1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20076,7 +20076,7 @@
         <v>173</v>
       </c>
       <c r="C1" s="30" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -20106,40 +20106,46 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c r="C7" s="24"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
+        <v>251</v>
+      </c>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>179</v>
-      </c>
+      <c r="B10" s="23"/>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>204</v>
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-705: Add rule description on option for component QUALITY_TAGS_RULES_EVOLUTION
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6198D28-BF05-4E3D-BEC3-BC8B8A31A131}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E167DF1A-5772-4E51-8CF9-63E18F76CC6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="253">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -994,7 +994,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1171,14 +1171,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="16"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -1249,7 +1241,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1312,7 +1304,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1735,8 +1726,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1747,16 +1738,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -1804,26 +1795,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
+      <c r="G22" s="33"/>
+      <c r="H22" s="33"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -1863,7 +1854,7 @@
       <c r="B1" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>248</v>
       </c>
     </row>
@@ -2000,7 +1991,7 @@
       </c>
     </row>
     <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2010,7 +2001,7 @@
       </c>
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>249</v>
       </c>
     </row>
@@ -2377,9 +2368,9 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
-  <dimension ref="B1:C10"/>
+  <dimension ref="B1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2388,11 +2379,13 @@
     <col min="2" max="2" width="90.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="29" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
@@ -2410,26 +2403,31 @@
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
+      <c r="B5" s="23" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>179</v>
-      </c>
+      <c r="B6" s="23"/>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-    </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B9" s="23"/>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="22"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2457,7 +2455,7 @@
       <c r="B1" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="30"/>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
@@ -20062,8 +20060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
   <dimension ref="B1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20075,7 +20073,7 @@
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="29" t="s">
         <v>248</v>
       </c>
     </row>

</xml_diff>

<commit_message>
REPORTGEN-704: update excel report template with LIST_RULE_VIOLATIONS_BOOKMARKS_TABLE
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E167DF1A-5772-4E51-8CF9-63E18F76CC6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F301003-331E-424E-9907-2C1BD0D8ABD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="8" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -31,6 +31,7 @@
     <sheet name="3 - AETP list" sheetId="24" r:id="rId16"/>
     <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId17"/>
     <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId18"/>
+    <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="260">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -985,6 +986,27 @@
   </si>
   <si>
     <t>* DESC=true|false. For display rationale, description and remediation of the rule. By default if not present, it is false</t>
+  </si>
+  <si>
+    <t>3.16.	Evolution of CAST rules associated to a quality standard category</t>
+  </si>
+  <si>
+    <t>3.17.	List of violations with bookmarks without source code for a list of rules</t>
+  </si>
+  <si>
+    <t>* Block Name = LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE</t>
+  </si>
+  <si>
+    <t>* COUNT=N where N indicates the top number of violations ; by default 5 (-1 correspond to all violations). All bookmarks of a violation are displayed.</t>
+  </si>
+  <si>
+    <t>To use the quality standard tags selection, the Quality Standards Support extension should be installed on the central where the application resides, with minimum version 20190624.</t>
+  </si>
+  <si>
+    <t>This component is only relevant for excel document. The results would not be readable on powerpoint or word.</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=CISQ-Security,COUNT=-1</t>
   </si>
 </sst>
 </file>
@@ -2370,7 +2392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
   <dimension ref="B1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2442,7 +2464,7 @@
   <dimension ref="B1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2453,7 +2475,7 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="C1" s="29"/>
     </row>
@@ -2496,6 +2518,88 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
+  <dimension ref="B1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="28"/>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
REPORTGEN-708: Add No Header option for components in excel reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F301003-331E-424E-9907-2C1BD0D8ABD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFF6140-008E-447F-9CFF-8A5F817D1BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" firstSheet="10" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="701" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="263">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1007,6 +1007,15 @@
   </si>
   <si>
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=CISQ-Security,COUNT=-1</t>
+  </si>
+  <si>
+    <t>* EVOLUTION=true|false to display added and removed violations columns. By default or if not exists, is true if there is a previous snapshot.</t>
+  </si>
+  <si>
+    <t>* HEADER=NO to not display headers (useful for excel report when you want to define your own customized headers). By default if option is not present or different from NO, headers are displayed</t>
+  </si>
+  <si>
+    <t>NEW</t>
   </si>
 </sst>
 </file>
@@ -1729,29 +1738,29 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="36.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="36.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
     </row>
-    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1759,7 +1768,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="3"/>
@@ -1767,7 +1776,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="3"/>
@@ -1775,54 +1784,54 @@
       <c r="F4" s="1"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="17"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="17" t="s">
         <v>77</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C13" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
@@ -1830,7 +1839,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -1838,7 +1847,7 @@
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E23" s="12"/>
       <c r="F23" s="11"/>
     </row>
@@ -1861,18 +1870,18 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
-  <dimension ref="B1:C11"/>
+  <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>232</v>
       </c>
@@ -1880,47 +1889,57 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="23" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="22"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
         <v>185</v>
       </c>
     </row>
@@ -1938,101 +1957,101 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="22"/>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="30" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>250</v>
       </c>
@@ -2051,51 +2070,51 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>202</v>
       </c>
@@ -2114,52 +2133,52 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>204</v>
       </c>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="27" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="22"/>
     </row>
   </sheetData>
@@ -2176,86 +2195,86 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="24" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="20" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" s="24"/>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" s="25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" s="25" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" s="25" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="25" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>226</v>
       </c>
@@ -2274,56 +2293,56 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="22"/>
     </row>
   </sheetData>
@@ -2340,46 +2359,46 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23"/>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
     </row>
   </sheetData>
@@ -2390,18 +2409,18 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
-  <dimension ref="B1:C11"/>
+  <dimension ref="B1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>239</v>
       </c>
@@ -2409,47 +2428,52 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B9" s="23" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="23"/>
+    </row>
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
         <v>238</v>
       </c>
     </row>
@@ -2467,51 +2491,51 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
-    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="3" max="3" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>253</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23"/>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23"/>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="22"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>243</v>
       </c>
@@ -2525,74 +2549,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
   <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
-    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="3" max="3" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C1" s="29" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="28"/>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>259</v>
       </c>
@@ -2611,643 +2639,643 @@
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" style="18" customWidth="1"/>
     <col min="6" max="7" width="38" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="18"/>
-    <col min="11" max="11" width="14.28515625" style="18" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="18" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="18"/>
+    <col min="8" max="8" width="11.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="18"/>
+    <col min="11" max="11" width="14.33203125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="36.6640625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="18" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B23" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B33" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B38" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B43" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B48" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B53" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B58" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B63" s="19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B73" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B78" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B83" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B88" s="19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B95" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B102" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B109" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B114" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B119" s="19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B124" s="19" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B129" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B134" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B143" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B144" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B145" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B146" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B147" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B148" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B149" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="18" t="s">
         <v>119</v>
       </c>
@@ -3266,19 +3294,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -3286,7 +3314,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -3294,7 +3322,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -3302,7 +3330,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -3320,32 +3348,32 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="36.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>60</v>
       </c>
@@ -3353,7 +3381,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>62</v>
       </c>
@@ -3361,7 +3389,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>64</v>
       </c>
@@ -3369,19 +3397,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3404,22 +3432,22 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>82</v>
       </c>
@@ -3427,7 +3455,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>83</v>
       </c>
@@ -3435,7 +3463,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>84</v>
       </c>
@@ -3443,7 +3471,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>85</v>
       </c>
@@ -3451,7 +3479,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>86</v>
       </c>
@@ -3459,7 +3487,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>87</v>
       </c>
@@ -3467,7 +3495,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>88</v>
       </c>
@@ -3475,7 +3503,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>89</v>
       </c>
@@ -3483,7 +3511,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>90</v>
       </c>
@@ -3491,7 +3519,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>102</v>
       </c>
@@ -3499,8 +3527,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>101</v>
       </c>
@@ -3518,92 +3546,92 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>146</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>164</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>150</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
         <v>148</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="22"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3622,47 +3650,47 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16384" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>171</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>153</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>154</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -20048,35 +20076,35 @@
       <c r="XFC6" s="22"/>
       <c r="XFD6" s="22"/>
     </row>
-    <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>156</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -20095,62 +20123,62 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>160</v>
       </c>
@@ -20162,18 +20190,18 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
-  <dimension ref="B1:C15"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
@@ -20181,72 +20209,78 @@
         <v>248</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>233</v>
       </c>
       <c r="C7" s="24"/>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>251</v>
       </c>
       <c r="C8" s="24"/>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>252</v>
       </c>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="23" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
+    <row r="13" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+    <row r="14" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+    <row r="15" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="22"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
         <v>203</v>
       </c>
     </row>

</xml_diff>

<commit_message>
BUILD-0000: update reports for 1.15.0
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFF6140-008E-447F-9CFF-8A5F817D1BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552380B0-80B1-4766-B531-142E1A21EB08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="701" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="261">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -973,9 +973,6 @@
     <t>GREATER2 : components should have prop2 value greater than this value</t>
   </si>
   <si>
-    <t>UPDATED</t>
-  </si>
-  <si>
     <t>When using LOWER and GREATER parameters, the ORDER parameter can be overridden to get the most accurate components corresponding to the request. As the filter can be done only after requesting data from the RestAPI, the list can be truncated. So the option NBSET define the number of objects returns from the rest api before the filtering and the limitation of display (COUNT), this option is set to 500 by default, to avoid too long server response time.</t>
   </si>
   <si>
@@ -1013,9 +1010,6 @@
   </si>
   <si>
     <t>* HEADER=NO to not display headers (useful for excel report when you want to define your own customized headers). By default if option is not present or different from NO, headers are displayed</t>
-  </si>
-  <si>
-    <t>NEW</t>
   </si>
 </sst>
 </file>
@@ -1734,33 +1728,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1768,7 +1762,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="3"/>
@@ -1776,7 +1770,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="3"/>
@@ -1784,54 +1778,54 @@
       <c r="F4" s="1"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="17"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="10" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>77</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="13" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
@@ -1839,7 +1833,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -1847,7 +1841,7 @@
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
       <c r="F23" s="11"/>
     </row>
@@ -1873,72 +1867,70 @@
   <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23"/>
     </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>185</v>
       </c>
@@ -1957,103 +1949,103 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="22"/>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2070,51 +2062,51 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>202</v>
       </c>
@@ -2133,52 +2125,52 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>204</v>
       </c>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
     </row>
   </sheetData>
@@ -2195,86 +2187,86 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="24"/>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>226</v>
       </c>
@@ -2293,56 +2285,56 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
     </row>
   </sheetData>
@@ -2359,46 +2351,46 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23"/>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
     </row>
   </sheetData>
@@ -2415,64 +2407,62 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23"/>
     </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>238</v>
       </c>
@@ -2491,51 +2481,51 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
-    <col min="3" max="3" width="109.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23"/>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23"/>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>243</v>
       </c>
@@ -2550,79 +2540,77 @@
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
-    <col min="3" max="3" width="109.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
         <v>254</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2635,647 +2623,647 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B150"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B62" sqref="B62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="18" customWidth="1"/>
     <col min="6" max="7" width="38" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="18"/>
-    <col min="11" max="11" width="14.33203125" style="18" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" style="18" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="18"/>
+    <col min="8" max="8" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="18"/>
+    <col min="11" max="11" width="14.28515625" style="18" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="18" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B53" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B58" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B63" s="19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B73" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B78" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B83" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B88" s="19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B95" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B102" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B109" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B114" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B119" s="19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B124" s="19" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B129" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B134" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B143" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B144" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B145" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B146" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B147" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B148" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B149" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="18" t="s">
         <v>119</v>
       </c>
@@ -3294,19 +3282,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -3314,7 +3302,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -3322,7 +3310,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -3330,7 +3318,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -3348,32 +3336,32 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>60</v>
       </c>
@@ -3381,7 +3369,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>62</v>
       </c>
@@ -3389,7 +3377,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>64</v>
       </c>
@@ -3397,19 +3385,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3432,22 +3420,22 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>82</v>
       </c>
@@ -3455,7 +3443,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>83</v>
       </c>
@@ -3463,7 +3451,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>84</v>
       </c>
@@ -3471,7 +3459,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>85</v>
       </c>
@@ -3479,7 +3467,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>86</v>
       </c>
@@ -3487,7 +3475,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>87</v>
       </c>
@@ -3495,7 +3483,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>88</v>
       </c>
@@ -3503,7 +3491,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>89</v>
       </c>
@@ -3511,7 +3499,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>90</v>
       </c>
@@ -3519,7 +3507,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>102</v>
       </c>
@@ -3527,8 +3515,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>101</v>
       </c>
@@ -3546,92 +3534,92 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>146</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>164</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>150</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>148</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3650,47 +3638,47 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>171</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>153</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>154</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -20076,35 +20064,35 @@
       <c r="XFC6" s="22"/>
       <c r="XFD6" s="22"/>
     </row>
-    <row r="7" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>156</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -20123,62 +20111,62 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>160</v>
       </c>
@@ -20192,94 +20180,92 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
   <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>233</v>
       </c>
       <c r="C7" s="24"/>
     </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>252</v>
-      </c>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="24"/>
     </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23"/>
     </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
REPORTGEN-782: add MODULE and TECHNO options, update library reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{552380B0-80B1-4766-B531-142E1A21EB08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D6B41-8536-4474-9A23-AA67A7DFEAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="28800" windowHeight="15435" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="-12840" windowWidth="21600" windowHeight="11325" tabRatio="701" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -42,12 +42,22 @@
     <definedName name="TABLE_4" comment="TEXT;LAST_SNAPSHOT_DATE" localSheetId="0">'1 - Information'!$D$4:$D$4</definedName>
     <definedName name="TABLE_5" comment="TEXT;TODAY_DATE" localSheetId="0">'1 - Information'!$F$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="272">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1010,6 +1020,39 @@
   </si>
   <si>
     <t>* HEADER=NO to not display headers (useful for excel report when you want to define your own customized headers). By default if option is not present or different from NO, headers are displayed</t>
+  </si>
+  <si>
+    <t>2.26. - Metric Evolution</t>
+  </si>
+  <si>
+    <t>This component display the evolution of a metric, in percentage or in absolute, for the application, or for a module or a technology if specified.</t>
+  </si>
+  <si>
+    <t>* Block Name = METRIC_EVOLUTION</t>
+  </si>
+  <si>
+    <t>- ID=can be quality indicator ID (BC, TC or QR), or sizing measure, or background fact. Mandatory parameter</t>
+  </si>
+  <si>
+    <t>- FORMAT=ABSOLUTE or PERCENT to get the variation either direct value, either percentage. Default is percent. (optional)</t>
+  </si>
+  <si>
+    <t>If no module and no technology this is the value for the application that is taken.</t>
+  </si>
+  <si>
+    <t>Variation in percent = (current - previous) / previous</t>
+  </si>
+  <si>
+    <t>Variation in absolute = current - previous</t>
+  </si>
+  <si>
+    <t>- MODULE=name of the module for which you want the metric evolution (optional)</t>
+  </si>
+  <si>
+    <t>- TECHNO=name of the technology for which you want the metric evolution (optional)</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;METRIC_EVOLUTION;ID=60017</t>
   </si>
 </sst>
 </file>
@@ -1728,33 +1771,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
-    <col min="2" max="2" width="6.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="36.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="36.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
     </row>
-    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1762,7 +1805,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="3"/>
@@ -1770,7 +1813,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="3"/>
@@ -1778,54 +1821,54 @@
       <c r="F4" s="1"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="17"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C11" s="17" t="s">
         <v>77</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C13" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
@@ -1833,7 +1876,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -1841,7 +1884,7 @@
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
       <c r="E23" s="12"/>
       <c r="F23" s="11"/>
     </row>
@@ -1870,67 +1913,67 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>232</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="23"/>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>185</v>
       </c>
@@ -1949,101 +1992,101 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="22"/>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="30" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="30" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>249</v>
       </c>
@@ -2062,51 +2105,51 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>202</v>
       </c>
@@ -2125,52 +2168,52 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>204</v>
       </c>
       <c r="I1" s="26"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="27" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="22"/>
     </row>
   </sheetData>
@@ -2187,86 +2230,86 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="20" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="24" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="20" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="20" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="20" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="20" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" s="24"/>
     </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B12" s="25" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" s="25" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" s="25" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="25" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>226</v>
       </c>
@@ -2285,56 +2328,56 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="22"/>
     </row>
   </sheetData>
@@ -2351,46 +2394,46 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="11" max="12" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23"/>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
     </row>
   </sheetData>
@@ -2407,62 +2450,62 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>239</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="23"/>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="22"/>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>238</v>
       </c>
@@ -2481,51 +2524,51 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
-    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="3" max="3" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>252</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23"/>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23"/>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="22"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>243</v>
       </c>
@@ -2543,72 +2586,72 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
-    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="3" max="3" width="109.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>253</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="28" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="28" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="28" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>258</v>
       </c>
@@ -2621,651 +2664,711 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:B150"/>
+  <dimension ref="B2:B163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="B163" sqref="B163"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="18" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="18" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" style="18" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" style="18" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" style="18" customWidth="1"/>
     <col min="6" max="7" width="38" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="18"/>
-    <col min="11" max="11" width="14.28515625" style="18" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" style="18" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="18"/>
+    <col min="8" max="8" width="11.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.109375" style="18"/>
+    <col min="11" max="11" width="14.33203125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="36.6640625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" style="18" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B18" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B23" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B28" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B33" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B38" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B43" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B48" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B53" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B58" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" s="21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B63" s="19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" s="21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B73" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B74" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B75" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B76" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B78" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B79" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B80" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B83" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B88" s="19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B95" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B96" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B97" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B98" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B99" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B100" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B102" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B103" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B104" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B105" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B106" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B107" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B109" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B110" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B111" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B112" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B114" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B115" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B116" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B117" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B119" s="19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B120" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B121" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B122" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B124" s="19" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B125" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B126" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B127" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B129" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B130" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B131" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B132" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B134" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B135" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B136" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B137" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B138" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B139" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B140" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B141" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B142" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B143" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B144" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B145" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B146" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B147" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B148" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B149" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="18" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="B152" s="19" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B153" s="18" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B154" s="18" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B155" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B156" s="21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B157" s="21" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B158" s="21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B159" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B160" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B161" s="18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B162" s="18" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B163" s="18" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3282,19 +3385,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -3302,7 +3405,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -3310,7 +3413,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -3318,7 +3421,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -3336,32 +3439,32 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="35.44140625" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="36.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>60</v>
       </c>
@@ -3369,7 +3472,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>62</v>
       </c>
@@ -3377,7 +3480,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>64</v>
       </c>
@@ -3385,19 +3488,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3420,22 +3523,22 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>82</v>
       </c>
@@ -3443,7 +3546,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="18" t="s">
         <v>83</v>
       </c>
@@ -3451,7 +3554,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="18" t="s">
         <v>84</v>
       </c>
@@ -3459,7 +3562,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>85</v>
       </c>
@@ -3467,7 +3570,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B7" s="18" t="s">
         <v>86</v>
       </c>
@@ -3475,7 +3578,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>87</v>
       </c>
@@ -3483,7 +3586,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>88</v>
       </c>
@@ -3491,7 +3594,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>89</v>
       </c>
@@ -3499,7 +3602,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>90</v>
       </c>
@@ -3507,7 +3610,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>102</v>
       </c>
@@ -3515,8 +3618,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>101</v>
       </c>
@@ -3534,92 +3637,92 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>146</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>164</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>150</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="22" t="s">
         <v>148</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="22"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3638,47 +3741,47 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16384" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>171</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>153</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>154</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -20064,35 +20167,35 @@
       <c r="XFC6" s="22"/>
       <c r="XFD6" s="22"/>
     </row>
-    <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>156</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -20111,62 +20214,62 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>160</v>
       </c>
@@ -20184,88 +20287,88 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="18" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>233</v>
       </c>
       <c r="C7" s="24"/>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
         <v>250</v>
       </c>
       <c r="C8" s="24"/>
     </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
         <v>251</v>
       </c>
       <c r="C9" s="24"/>
     </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>260</v>
       </c>
       <c r="C10" s="24"/>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="23"/>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="22"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
REPORTGEN-871: update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19D6B41-8536-4474-9A23-AA67A7DFEAAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BFE72C-EC8D-4475-883F-3BA5EB3D4C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="-12840" windowWidth="21600" windowHeight="11325" tabRatio="701" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -585,9 +585,6 @@
     <t>* Block Name = RULES_LIST_STATISTICS_RATIO</t>
   </si>
   <si>
-    <t>* METRICS=List of metrics id (BC, TC or QR) or quality standards tags separated by ‘|’.</t>
-  </si>
-  <si>
     <t>* CRITICAL=true : add this option if you have selected a BC or a TC and want only critical rules to be selected (by default it is false). This option has no effect on selection by QR or quality standard tag.</t>
   </si>
   <si>
@@ -1053,6 +1050,9 @@
   </si>
   <si>
     <t>RepGen:TEXT;METRIC_EVOLUTION;ID=60017</t>
+  </si>
+  <si>
+    <t>* METRICS=List of metrics id (BC, TC or QR) or quality standards tags separated by ‘|’. It can also be the name for a BC or a shortName for a TC</t>
   </si>
 </sst>
 </file>
@@ -1775,29 +1775,29 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
       <c r="F1" s="32"/>
       <c r="G1" s="32"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -1805,7 +1805,7 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="3"/>
@@ -1813,7 +1813,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
       <c r="D4" s="3"/>
@@ -1821,54 +1821,54 @@
       <c r="F4" s="1"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="17"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="17" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="9"/>
     </row>
-    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="9"/>
     </row>
-    <row r="10" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="17" t="s">
         <v>6</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="17" t="s">
         <v>77</v>
       </c>
       <c r="N11" s="3"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="13" spans="2:15" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="17" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C20" s="35"/>
       <c r="D20" s="35"/>
       <c r="E20" s="35"/>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
@@ -1876,7 +1876,7 @@
       <c r="G21" s="33"/>
       <c r="H21" s="33"/>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
       <c r="E22" s="31"/>
@@ -1884,7 +1884,7 @@
       <c r="G22" s="33"/>
       <c r="H22" s="33"/>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
       <c r="F23" s="11"/>
     </row>
@@ -1913,69 +1913,69 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="22"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1992,103 +1992,103 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="30" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="30" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="12" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="27" t="s">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="15" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="30" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="30" t="s">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
         <v>248</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2105,53 +2105,53 @@
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="22"/>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="22"/>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2168,52 +2168,52 @@
       <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="I1" s="26"/>
+    </row>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>204</v>
       </c>
-      <c r="I1" s="26"/>
-    </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="5" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
     </row>
   </sheetData>
@@ -2230,88 +2230,88 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="24" t="s">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="20" t="s">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="20" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="20" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="25" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="25" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="25" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B12" s="25" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B13" s="25" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>225</v>
-      </c>
-    </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B14" s="25" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B15" s="25" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2328,56 +2328,56 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="18" t="s">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="18" t="s">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23"/>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22"/>
     </row>
   </sheetData>
@@ -2394,46 +2394,46 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="11" max="12" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23"/>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
     </row>
   </sheetData>
@@ -2450,64 +2450,64 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23"/>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>237</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23"/>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="22"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2524,53 +2524,53 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
-    <col min="3" max="3" width="109.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="23"/>
-    </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23"/>
-    </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>242</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="22"/>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2582,78 +2582,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
   <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="90.33203125" customWidth="1"/>
-    <col min="3" max="3" width="109.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="28" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="28" t="s">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>257</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -2666,709 +2666,709 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="18" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="18" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" style="18" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="18" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="18" customWidth="1"/>
     <col min="6" max="7" width="38" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" style="18" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.109375" style="18"/>
-    <col min="11" max="11" width="14.33203125" style="18" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" style="18" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" style="18" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="18"/>
+    <col min="8" max="8" width="11.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="18"/>
+    <col min="11" max="11" width="14.28515625" style="18" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" style="18" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" style="18" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="19" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B28" s="19" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B33" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="18" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B38" s="19" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B43" s="19" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" s="18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B48" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="18" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="18" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B53" s="19" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="18" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B58" s="19" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B63" s="19" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="18" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="73" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B73" s="19" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B78" s="19" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="83" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B83" s="19" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="18" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="88" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B88" s="19" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="95" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B95" s="19" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="18" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B102" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B103" s="18" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="18" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="109" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B109" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="18" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="114" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B114" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="18" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="119" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B119" s="19" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="18" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="2:2" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B124" s="19" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="18" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="129" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B129" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="18" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B131" s="18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B132" s="18" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="134" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B134" s="19" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="18" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B136" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B137" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="18" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="18" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B143" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B144" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B145" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B146" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B147" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B148" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B149" s="20" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B150" s="18" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="152" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B152" s="19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" s="18" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B153" s="18" t="s">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" s="18" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B154" s="18" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="18" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" s="21" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B157" s="21" t="s">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" s="21" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" s="21" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" s="18" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B158" s="21" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B159" s="21" t="s">
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161" s="18" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162" s="18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163" s="18" t="s">
         <v>270</v>
-      </c>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B160" s="18" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B161" s="18" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="162" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B162" s="18" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="163" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B163" s="18" t="s">
-        <v>271</v>
       </c>
     </row>
   </sheetData>
@@ -3385,19 +3385,19 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>70</v>
       </c>
@@ -3405,7 +3405,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>71</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>72</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>75</v>
       </c>
@@ -3439,32 +3439,32 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="35.44140625" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.42578125" customWidth="1"/>
     <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
-    <col min="12" max="12" width="36.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.88671875" customWidth="1"/>
+    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:8" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>60</v>
       </c>
@@ -3472,7 +3472,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>62</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>64</v>
       </c>
@@ -3488,19 +3488,19 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="15"/>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -3523,22 +3523,22 @@
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" s="19" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:3" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>82</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>83</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>84</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>85</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>86</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>87</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>88</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>89</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>90</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>102</v>
       </c>
@@ -3618,8 +3618,8 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:3" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>101</v>
       </c>
@@ -3637,92 +3637,92 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>146</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>147</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>149</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>164</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>150</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
-    <row r="7" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>152</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
         <v>148</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="2:4" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>169</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3741,47 +3741,47 @@
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>171</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>153</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
         <v>154</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
-    <row r="4" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>151</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="22"/>
       <c r="C6" s="22"/>
@@ -20167,35 +20167,35 @@
       <c r="XFC6" s="22"/>
       <c r="XFD6" s="22"/>
     </row>
-    <row r="7" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>165</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
     </row>
-    <row r="8" spans="1:16384" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>156</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B10" s="18"/>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
-    <row r="12" spans="1:16384" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -20214,62 +20214,62 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="92.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="8" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>160</v>
       </c>
@@ -20284,93 +20284,93 @@
   <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="121.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="23" t="s">
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="23" t="s">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="23" t="s">
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="24"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="23" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" s="24"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
-        <v>251</v>
-      </c>
-      <c r="C9" s="24"/>
-    </row>
-    <row r="10" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="C10" s="24"/>
-    </row>
-    <row r="11" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="23" t="s">
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="23" t="s">
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="22"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-877: update library component templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BFE72C-EC8D-4475-883F-3BA5EB3D4C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBD6B28-F1A5-49EA-BE12-6C36E0383DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="12" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="273">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -944,9 +944,6 @@
     <t>* Block Name = QUALITY_TAGS_RULES_EVOLUTION</t>
   </si>
   <si>
-    <t>* STD= Name of the quality standard category for which you want the details per tag, for example, STIG-V4R8-CAT1 will list total, added and removed violations for cast rules associated to all tags belonged to category STIG-V4R8-CAT1</t>
-  </si>
-  <si>
     <t>To use this component, the Quality Standards Mapping extension should be installed on the central where the application resides, with minimum version 20190624</t>
   </si>
   <si>
@@ -1053,6 +1050,12 @@
   </si>
   <si>
     <t>* METRICS=List of metrics id (BC, TC or QR) or quality standards tags separated by ‘|’. It can also be the name for a BC or a shortName for a TC</t>
+  </si>
+  <si>
+    <t>UPDATED</t>
+  </si>
+  <si>
+    <t>* STD= Name of the quality standard category, or BC name, or BC id, for which you want the details per tag or TC, for example, STIG-V4R8-CAT1 will list total, added and removed violations for cast rules associated to all tags belonged to category STIG-V4R8-CAT1</t>
   </si>
 </sst>
 </file>
@@ -1946,12 +1949,12 @@
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2035,22 +2038,22 @@
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2078,7 +2081,7 @@
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -2088,7 +2091,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2446,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2457,9 +2460,11 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="C1" s="29"/>
+        <v>237</v>
+      </c>
+      <c r="C1" s="29" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
@@ -2468,7 +2473,7 @@
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>235</v>
+        <v>272</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2478,12 +2483,12 @@
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2496,7 +2501,7 @@
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2507,7 +2512,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2532,18 +2537,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2559,7 +2564,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2570,7 +2575,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2582,7 +2587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
   <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2594,18 +2599,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2615,12 +2620,12 @@
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2638,12 +2643,12 @@
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2653,7 +2658,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -3313,17 +3318,17 @@
     </row>
     <row r="152" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B152" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="153" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B153" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
@@ -3333,42 +3338,42 @@
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B156" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -20284,7 +20289,7 @@
   <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20296,7 +20301,9 @@
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="29" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
@@ -20305,7 +20312,7 @@
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -20331,19 +20338,19 @@
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C8" s="24"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C9" s="24"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C10" s="24"/>
     </row>

</xml_diff>

<commit_message>
REPORTGEN-885: update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBD6B28-F1A5-49EA-BE12-6C36E0383DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0333D-AFA8-4538-82D0-F07F0EBCDFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11325" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="274">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1056,6 +1056,9 @@
   </si>
   <si>
     <t>* STD= Name of the quality standard category, or BC name, or BC id, for which you want the details per tag or TC, for example, STIG-V4R8-CAT1 will list total, added and removed violations for cast rules associated to all tags belonged to category STIG-V4R8-CAT1</t>
+  </si>
+  <si>
+    <t>The STD parameter can also take the name, shortName or ID os a Business Criterion</t>
   </si>
 </sst>
 </file>
@@ -1774,7 +1777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1910,10 +1913,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
-  <dimension ref="B1:C13"/>
+  <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,7 +1928,9 @@
       <c r="B1" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="29" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
@@ -1938,46 +1943,51 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>232</v>
+      <c r="B4" s="28" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-    </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>178</v>
-      </c>
+      <c r="B9" s="23"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-    </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>184</v>
       </c>
     </row>
@@ -2449,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
REPORTGEN-0000 : update library template reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29D0333D-AFA8-4538-82D0-F07F0EBCDFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0164B4E3-CBF3-4B85-9799-0EE57D79EB0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11325" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="273">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1050,9 +1050,6 @@
   </si>
   <si>
     <t>* METRICS=List of metrics id (BC, TC or QR) or quality standards tags separated by ‘|’. It can also be the name for a BC or a shortName for a TC</t>
-  </si>
-  <si>
-    <t>UPDATED</t>
   </si>
   <si>
     <t>* STD= Name of the quality standard category, or BC name, or BC id, for which you want the details per tag or TC, for example, STIG-V4R8-CAT1 will list total, added and removed violations for cast rules associated to all tags belonged to category STIG-V4R8-CAT1</t>
@@ -1916,7 +1913,7 @@
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1928,9 +1925,7 @@
       <c r="B1" s="19" t="s">
         <v>231</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>271</v>
-      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
@@ -1944,7 +1939,7 @@
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2472,9 +2467,7 @@
       <c r="B1" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>271</v>
-      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
@@ -2483,7 +2476,7 @@
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -20311,9 +20304,7 @@
       <c r="B1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="29" t="s">
-        <v>271</v>
-      </c>
+      <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">

</xml_diff>

<commit_message>
REPORTGEN-914: update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0164B4E3-CBF3-4B85-9799-0EE57D79EB0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935EE5A5-3902-4263-A1C9-5FD8C7391569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -56,6 +56,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="273">
   <si>
@@ -375,9 +397,6 @@
   </si>
   <si>
     <t xml:space="preserve">* Options = </t>
-  </si>
-  <si>
-    <t>- PARAMS=SZ a SZ b, (SZ pour sizing measure, QR pour quality rule, BF for background fact)</t>
   </si>
   <si>
     <t>- EXPR=b/a, (operators can be +, -, *, / , (, ) )</t>
@@ -1056,6 +1075,9 @@
   </si>
   <si>
     <t>The STD parameter can also take the name, shortName or ID os a Business Criterion</t>
+  </si>
+  <si>
+    <t>You can put a category id instead of a sizing measure, for example 65104 for  very large size artifact.</t>
   </si>
 </sst>
 </file>
@@ -1923,43 +1945,43 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1967,12 +1989,12 @@
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1983,7 +2005,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2008,62 +2030,62 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2071,32 +2093,32 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>
@@ -2121,37 +2143,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2159,7 +2181,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2184,33 +2206,33 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2218,7 +2240,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2246,52 +2268,52 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2299,27 +2321,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2344,37 +2366,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2382,7 +2404,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2410,27 +2432,27 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2438,7 +2460,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2465,33 +2487,33 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2499,12 +2521,12 @@
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2515,7 +2537,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2540,18 +2562,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2562,12 +2584,12 @@
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2578,7 +2600,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2602,33 +2624,33 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2636,32 +2658,32 @@
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -2672,10 +2694,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:B163"/>
+  <dimension ref="B2:B164"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="B152" sqref="B152"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="G151" sqref="G151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2731,7 +2753,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2771,7 +2793,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -2931,62 +2953,62 @@
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B63" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B73" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
@@ -3006,7 +3028,7 @@
     </row>
     <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B78" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
@@ -3026,7 +3048,7 @@
     </row>
     <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B83" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
@@ -3046,7 +3068,7 @@
     </row>
     <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B88" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
@@ -3061,22 +3083,22 @@
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B95" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
@@ -3091,22 +3113,22 @@
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B102" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
@@ -3121,22 +3143,22 @@
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B109" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
@@ -3156,7 +3178,7 @@
     </row>
     <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B114" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
@@ -3176,7 +3198,7 @@
     </row>
     <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B119" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
@@ -3196,7 +3218,7 @@
     </row>
     <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B124" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
@@ -3216,7 +3238,7 @@
     </row>
     <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B129" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
@@ -3236,7 +3258,7 @@
     </row>
     <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B134" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
@@ -3250,133 +3272,139 @@
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="18" t="s">
-        <v>106</v>
+      <c r="B137" s="18" t="e" cm="1">
+        <f t="array" ref="B137">- PARAMS=SZ a SZ b, (SZ pour sizing measure or category, QR pour quality rule, BF for background fact)</f>
+        <v>#NAME?</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B139" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B140" s="18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="18" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B143" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B144" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B145" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B146" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B147" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B148" s="20" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B149" s="20" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B150" s="20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" s="18" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B150" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="152" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B152" s="19" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B153" s="18" t="s">
-        <v>260</v>
+    <row r="153" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B153" s="19" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="18" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" s="18" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="21" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="21" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="21" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="18" t="s">
-        <v>264</v>
+      <c r="B160" s="21" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B161" s="18" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="18" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="18" t="s">
-        <v>269</v>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="18" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3499,7 +3527,7 @@
     <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3652,49 +3680,49 @@
   <sheetData>
     <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3706,14 +3734,14 @@
     </row>
     <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
     <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -3725,7 +3753,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -3756,35 +3784,35 @@
   <sheetData>
     <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
@@ -20177,7 +20205,7 @@
     </row>
     <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -20189,7 +20217,7 @@
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -20229,57 +20257,57 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -20302,56 +20330,56 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C7" s="24"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C8" s="24"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C9" s="24"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C10" s="24"/>
     </row>
@@ -20360,17 +20388,17 @@
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -20378,7 +20406,7 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-915: update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{935EE5A5-3902-4263-A1C9-5FD8C7391569}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A0E033-0BF2-48BA-8EA1-7D5211B65836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,30 +56,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="275">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -400,12 +378,6 @@
   </si>
   <si>
     <t>- EXPR=b/a, (operators can be +, -, *, / , (, ) )</t>
-  </si>
-  <si>
-    <t>- a=67011,</t>
-  </si>
-  <si>
-    <t>- b=67010,</t>
   </si>
   <si>
     <t>- FORMAT=N0 (N2 by default, if nothing or erroneous format is set),</t>
@@ -1044,9 +1016,6 @@
     <t>* Block Name = METRIC_EVOLUTION</t>
   </si>
   <si>
-    <t>- ID=can be quality indicator ID (BC, TC or QR), or sizing measure, or background fact. Mandatory parameter</t>
-  </si>
-  <si>
     <t>- FORMAT=ABSOLUTE or PERCENT to get the variation either direct value, either percentage. Default is percent. (optional)</t>
   </si>
   <si>
@@ -1078,6 +1047,21 @@
   </si>
   <si>
     <t>You can put a category id instead of a sizing measure, for example 65104 for  very large size artifact.</t>
+  </si>
+  <si>
+    <t>- ID=can be quality indicator ID (BC, TC or QR), or sizing measure, or background fact, or category</t>
+  </si>
+  <si>
+    <t>- PARAMS=SZ a SZ b, (SZ pour sizing measure or category, QR pour quality rule, BF for background fact)</t>
+  </si>
+  <si>
+    <t>- a=id,</t>
+  </si>
+  <si>
+    <t>- b=id,</t>
+  </si>
+  <si>
+    <t>Either ID, either PARAMS and EXPR (for custom expression) should be specified</t>
   </si>
 </sst>
 </file>
@@ -1945,43 +1929,43 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1989,12 +1973,12 @@
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2005,7 +1989,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -2030,62 +2014,62 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2093,32 +2077,32 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2143,37 +2127,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2181,7 +2165,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2206,33 +2190,33 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2240,7 +2224,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2268,52 +2252,52 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2321,27 +2305,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2366,37 +2350,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2404,7 +2388,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2432,27 +2416,27 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2460,7 +2444,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2487,33 +2471,33 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2521,12 +2505,12 @@
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2537,7 +2521,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2562,18 +2546,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2584,12 +2568,12 @@
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2600,7 +2584,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -2624,33 +2608,33 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2658,32 +2642,32 @@
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -2694,10 +2678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:B164"/>
+  <dimension ref="B2:B169"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="G151" sqref="G151"/>
+    <sheetView topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2753,7 +2737,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2793,7 +2777,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -2953,62 +2937,62 @@
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B63" s="19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="18" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="21" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B73" s="19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
@@ -3028,7 +3012,7 @@
     </row>
     <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B78" s="19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
@@ -3048,7 +3032,7 @@
     </row>
     <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B83" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
@@ -3068,7 +3052,7 @@
     </row>
     <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B88" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
@@ -3083,22 +3067,22 @@
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B95" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
@@ -3113,22 +3097,22 @@
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B102" s="19" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="103" spans="2:2" x14ac:dyDescent="0.25">
@@ -3143,22 +3127,22 @@
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="21" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B109" s="19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
@@ -3178,7 +3162,7 @@
     </row>
     <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B114" s="19" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
@@ -3198,7 +3182,7 @@
     </row>
     <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B119" s="19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
@@ -3218,7 +3202,7 @@
     </row>
     <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B124" s="19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
@@ -3238,7 +3222,7 @@
     </row>
     <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B129" s="19" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
@@ -3258,7 +3242,7 @@
     </row>
     <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B134" s="19" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
@@ -3272,9 +3256,8 @@
       </c>
     </row>
     <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="18" t="e" cm="1">
-        <f t="array" ref="B137">- PARAMS=SZ a SZ b, (SZ pour sizing measure or category, QR pour quality rule, BF for background fact)</f>
-        <v>#NAME?</v>
+      <c r="B137" s="21" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
@@ -3283,83 +3266,83 @@
       </c>
     </row>
     <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="18" t="s">
-        <v>107</v>
+      <c r="B139" s="21" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="18" t="s">
-        <v>108</v>
+      <c r="B140" s="21" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="141" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B141" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="142" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B142" s="18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B143" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B144" s="20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B145" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B146" s="20" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B147" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B148" s="20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B149" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="150" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B150" s="20" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="151" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B151" s="18" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="153" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B153" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="154" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B154" s="18" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="155" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B155" s="18" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="156" spans="2:2" x14ac:dyDescent="0.25">
@@ -3369,42 +3352,67 @@
     </row>
     <row r="157" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B157" s="21" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="158" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B158" s="21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B159" s="21" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="160" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B160" s="21" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="18" t="s">
-        <v>263</v>
+      <c r="B161" s="21" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="18" t="s">
-        <v>264</v>
+        <v>106</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="18" t="s">
+      <c r="B163" s="21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" s="21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B165" s="21" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B166" s="18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="18" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B169" s="18" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="18" t="s">
-        <v>268</v>
       </c>
     </row>
   </sheetData>
@@ -3527,7 +3535,7 @@
     <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3680,49 +3688,49 @@
   <sheetData>
     <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3734,14 +3742,14 @@
     </row>
     <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
     <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -3753,7 +3761,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -3784,35 +3792,35 @@
   <sheetData>
     <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
@@ -20205,7 +20213,7 @@
     </row>
     <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -20217,7 +20225,7 @@
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -20257,57 +20265,57 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -20330,56 +20338,56 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C7" s="24"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C8" s="24"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C9" s="24"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C10" s="24"/>
     </row>
@@ -20388,17 +20396,17 @@
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -20406,7 +20414,7 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-916: update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3A0E033-0BF2-48BA-8EA1-7D5211B65836}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BECAC86-45EA-4614-B940-3C194624451A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="275">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -468,9 +468,6 @@
   </si>
   <si>
     <t>* Block Name = APPLICATION_METRIC</t>
-  </si>
-  <si>
-    <t>RepGen:TEXT;APPLICATION_METRIC;SZID=10151,SNAPSHOT=PREVIOUS,FORMAT=N0</t>
   </si>
   <si>
     <t>- RULID=quality rule id</t>
@@ -1062,6 +1059,9 @@
   </si>
   <si>
     <t>Either ID, either PARAMS and EXPR (for custom expression) should be specified</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;APPLICATION_METRIC;ID=10151,SNAPSHOT=PREVIOUS,FORMAT=N0</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1781,7 @@
   <dimension ref="B1:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1929,43 +1929,43 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1973,12 +1973,12 @@
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -1989,7 +1989,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2014,62 +2014,62 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2077,32 +2077,32 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2127,37 +2127,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2165,7 +2165,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2190,33 +2190,33 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2224,7 +2224,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2252,52 +2252,52 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2305,27 +2305,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2350,37 +2350,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2388,7 +2388,7 @@
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2416,27 +2416,27 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2444,7 +2444,7 @@
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2471,33 +2471,33 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2505,12 +2505,12 @@
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2546,18 +2546,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2568,12 +2568,12 @@
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2584,7 +2584,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2608,33 +2608,33 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2642,32 +2642,32 @@
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -2678,10 +2678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:B169"/>
+  <dimension ref="B2:B177"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="B166" sqref="B166"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2777,7 +2777,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -2937,12 +2937,12 @@
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
@@ -2986,433 +2986,473 @@
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B73" s="19" t="s">
-        <v>120</v>
+      <c r="B71" s="21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="21" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="18" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="18" t="s">
-        <v>31</v>
+      <c r="B75" s="21" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B78" s="19" t="s">
-        <v>121</v>
+      <c r="B76" s="21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="18" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="18" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B81" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="18" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="18" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B83" s="19" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="18" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B86" s="19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="18" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B88" s="19" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="21" t="s">
-        <v>138</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B91" s="19" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="21" t="s">
-        <v>139</v>
+      <c r="B92" s="18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B95" s="19" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="18" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B96" s="19" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B97" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="18" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="21" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="18" t="s">
+      <c r="B100" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="102" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B102" s="19" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="18" t="s">
-        <v>38</v>
+    <row r="103" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B103" s="19" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="18" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="21" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="18" t="s">
+      <c r="B107" s="21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="109" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B109" s="19" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="18" t="s">
-        <v>39</v>
+    <row r="110" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B110" s="19" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="18" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="112" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B112" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B114" s="19" t="s">
-        <v>127</v>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="21" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="18" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B116" s="18" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B117" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="18" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B117" s="18" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B119" s="19" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B121" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B122" s="19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="18" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B122" s="18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="124" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B124" s="19" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="18" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B126" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B127" s="19" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="18" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B127" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B129" s="19" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="130" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B130" s="18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B131" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B132" s="19" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" s="18" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B132" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="134" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B134" s="19" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="135" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B135" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B136" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="21" t="s">
-        <v>271</v>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B137" s="19" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B138" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B142" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143" s="18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" s="18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B139" s="21" t="s">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" s="21" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" s="21" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B140" s="21" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B141" s="18" t="s">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" s="18" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B142" s="18" t="s">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" s="18" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="143" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B143" s="20" t="s">
+    <row r="151" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B151" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="144" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B144" s="20" t="s">
+    <row r="152" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B152" s="20" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="145" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B145" s="20" t="s">
+    <row r="153" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B153" s="20" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="146" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B146" s="20" t="s">
+    <row r="154" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B154" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="147" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B147" s="20" t="s">
+    <row r="155" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B155" s="20" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="148" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B148" s="20" t="s">
+    <row r="156" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B156" s="20" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="149" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B149" s="20" t="s">
+    <row r="157" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B157" s="20" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="150" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B150" s="20" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B151" s="18" t="s">
+    <row r="158" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B158" s="20" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" s="18" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="153" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B153" s="19" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B154" s="18" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B155" s="18" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B156" s="18" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B157" s="21" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B158" s="21" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B159" s="21" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B160" s="21" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B161" s="21" t="s">
-        <v>271</v>
+    <row r="161" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B161" s="19" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="18" t="s">
-        <v>106</v>
+        <v>256</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B163" s="21" t="s">
-        <v>272</v>
+      <c r="B163" s="18" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B164" s="21" t="s">
-        <v>273</v>
+      <c r="B164" s="18" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="21" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B166" s="18" t="s">
+      <c r="B166" s="21" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B167" s="21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B168" s="21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B169" s="21" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B170" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B171" s="21" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B172" s="21" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B173" s="21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B174" s="18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B175" s="18" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="167" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B167" s="18" t="s">
+    <row r="176" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B176" s="18" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="168" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B168" s="18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="169" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B169" s="18" t="s">
-        <v>265</v>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B177" s="18" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -3535,7 +3575,7 @@
     <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3688,49 +3728,49 @@
   <sheetData>
     <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3742,14 +3782,14 @@
     </row>
     <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
     <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -3761,7 +3801,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -3792,35 +3832,35 @@
   <sheetData>
     <row r="1" spans="1:16384" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
@@ -20213,7 +20253,7 @@
     </row>
     <row r="7" spans="1:16384" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -20225,7 +20265,7 @@
     </row>
     <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
@@ -20265,57 +20305,57 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -20338,56 +20378,56 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="24"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C8" s="24"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C9" s="24"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C10" s="24"/>
     </row>
@@ -20396,17 +20436,17 @@
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -20414,7 +20454,7 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-969: commit changes after merge
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630DA43-D0AC-47CD-A21E-70665DF34221}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195D64C4-33FA-4F3F-A8AA-9CAE64659453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="9" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="280">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1071,6 +1071,12 @@
   </si>
   <si>
     <t>display the AFP value for previous snapshot (no by default)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Options : ZERO=YES|NO to </t>
+  </si>
+  <si>
+    <t>display the function with 0 AFP (yes by default)</t>
   </si>
 </sst>
 </file>
@@ -2347,7 +2353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B587AA6-980F-4560-B177-B792E0F411FE}">
   <dimension ref="B1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3534,10 +3540,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3597,26 +3603,34 @@
         <v>277</v>
       </c>
     </row>
-    <row r="7" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
+    <row r="7" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REPORTGEN-965 : update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195D64C4-33FA-4F3F-A8AA-9CAE64659453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4AC9AA-6173-46FF-95EB-9B259CAE07FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId17"/>
     <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId18"/>
     <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId19"/>
+    <sheet name="3-ActionPlanBookmarksTable" sheetId="28" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="285">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1077,6 +1078,21 @@
   </si>
   <si>
     <t>display the function with 0 AFP (yes by default)</t>
+  </si>
+  <si>
+    <t>3.18.	List of violations from action plan with bookmarks without source code</t>
+  </si>
+  <si>
+    <t>* Block Name = ACTION_PLAN_BOOKMARKS_TABLE</t>
+  </si>
+  <si>
+    <t>* COUNT=N where N indicates the top number of violations ; by default 5 (ALL correspond to all violations). All bookmarks of a violation are displayed.</t>
+  </si>
+  <si>
+    <t>* FILTER=added|pending|solved|all to filter the results with the remedial status of violations (all by default)</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;ACTION_PLAN_BOOKMARKS_TABLE;COUNT=-1</t>
   </si>
 </sst>
 </file>
@@ -2617,7 +2633,7 @@
   <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3481,6 +3497,69 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6A5E0-9666-42B8-820C-0803FCEF98B6}">
+  <dimension ref="B1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:C6"/>
@@ -3542,7 +3621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
REPORTGEN-994 & REPORTGEN-965: manage tag and priority columns for actions
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4AC9AA-6173-46FF-95EB-9B259CAE07FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91AA0B77-9C39-41EF-A8DA-FCB73FB77437}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="13" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="701" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId18"/>
     <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId19"/>
     <sheet name="3-ActionPlanBookmarksTable" sheetId="28" r:id="rId20"/>
+    <sheet name="Sheet1" sheetId="29" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="286">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1093,6 +1094,9 @@
   </si>
   <si>
     <t>RepGen:TABLE;ACTION_PLAN_BOOKMARKS_TABLE;COUNT=-1</t>
+  </si>
+  <si>
+    <t>* TAG=YES|NO, to display the priority using tag or priority (tag by default as this is this value that is set in ED)</t>
   </si>
 </sst>
 </file>
@@ -3499,10 +3503,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6A5E0-9666-42B8-820C-0803FCEF98B6}">
-  <dimension ref="B1:B11"/>
+  <dimension ref="B1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3533,29 +3537,47 @@
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
+      <c r="B6" s="23" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>174</v>
-      </c>
+      <c r="B7" s="23"/>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>220</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>284</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646BF52C-F02F-4980-9FBC-5E2F521BB50A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3937,10 +3959,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F8858A-750A-4726-A1F9-D59D03327DAC}">
-  <dimension ref="B1:D12"/>
+  <dimension ref="B1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3983,39 +4005,46 @@
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
-    <row r="6" spans="2:4" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="2:4" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-    </row>
-    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>152</v>
-      </c>
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="18"/>
+      <c r="B10" t="s">
+        <v>152</v>
+      </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
REPORTGEN-1053: update library and sizing templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A11332-B277-46F6-9C82-D8E513DEB76A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC19309-E6A7-459C-931A-40EF1FFD8E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="2505" windowWidth="21075" windowHeight="11385" tabRatio="701" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -31,9 +31,10 @@
     <sheet name="3 - AETP list" sheetId="24" r:id="rId16"/>
     <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId17"/>
     <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId18"/>
-    <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId19"/>
-    <sheet name="3-ActionPlanBookmarksTable" sheetId="28" r:id="rId20"/>
-    <sheet name="Sheet1" sheetId="29" r:id="rId21"/>
+    <sheet name="3-ActionPlanBookmarksTable" sheetId="28" r:id="rId19"/>
+    <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId20"/>
+    <sheet name="3-OMGTechDebt" sheetId="30" r:id="rId21"/>
+    <sheet name="3-OMGTechDebtDetails" sheetId="31" r:id="rId22"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="305">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -419,9 +420,6 @@
   </si>
   <si>
     <t>- SNAPSHOT=CURRENT | PREVIOUS (CURRENT by default)</t>
-  </si>
-  <si>
-    <t>2.14. - Technical Debt Result</t>
   </si>
   <si>
     <t>2.15. - Unadjusted Data Function Metric Value</t>
@@ -1101,6 +1099,86 @@
   <si>
     <t>FORMAT: The number of decimals for effort complexity, ratio and AETP count (N2 for 2 decimals, N5 for 5 decimals), by default N2.</t>
   </si>
+  <si>
+    <t>2.27. - OMG Technical Debt (based on a scope of rules)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.14. - Technical Debt Result </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Deprecated (old Cast formula)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, see new component in 2.27</t>
+    </r>
+  </si>
+  <si>
+    <t>This component display the OMG technical debt in Days related to the selected index : ISO, AIP or CISQ</t>
+  </si>
+  <si>
+    <t>ISO option is the recommended technical debt to be used. Requires installation of OMG Technical Debt Measure (&gt;2.0.0 funcrel) and ISO-5055 Index extensions during analysis</t>
+  </si>
+  <si>
+    <t>CISQ option required installation of OMG Technical Debt Measure and CISQ Index extensions during analysis. Scope of rules is reduced</t>
+  </si>
+  <si>
+    <t>* Block Name = OMG_TECHNICAL_DEBT</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;OMG_TECHNICAL_DEBT</t>
+  </si>
+  <si>
+    <t>* Options =</t>
+  </si>
+  <si>
+    <t>- ID:AIP|CISQ|ISO (by default or if nothing selected, ISO)</t>
+  </si>
+  <si>
+    <t>- SNAPSHOT:CURRENT|PREVIOUS (by default or if nothing, CURRENT)</t>
+  </si>
+  <si>
+    <t>3.18.	OMG Technical Debt (based on a scope of rules)</t>
+  </si>
+  <si>
+    <t>* Block Name = OMG_TECHNICAL_DEBT_TABLE</t>
+  </si>
+  <si>
+    <t>- HEADER:DAYS|SHORT (by default or if nothing selected, displays Days as unit and short name for OMG tech debt, or no unit if SHORT)</t>
+  </si>
+  <si>
+    <t>3.19.	OMG Technical Debt information on contributing TC</t>
+  </si>
+  <si>
+    <t>* Block Name = OMG_TECHNICAL_DEBT_DETAILS_TABLE</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_DETAILS_TABLE</t>
+  </si>
+  <si>
+    <t>If a TC has no omg technical debt, it will not be displayed in the table</t>
+  </si>
+  <si>
+    <t>This component can also display the list of rules for a TC (for that you can put the ID of the TC instead of AIP/CISQ or ISO)</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_TABLE</t>
+  </si>
 </sst>
 </file>
 
@@ -1109,7 +1187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1292,6 +1370,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1356,7 +1442,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1422,6 +1508,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1819,7 +1907,7 @@
   <dimension ref="B1:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,8 +1929,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -1853,16 +1941,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -1910,26 +1998,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="37"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -1967,43 +2055,43 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2011,12 +2099,12 @@
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2027,7 +2115,7 @@
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2052,62 +2140,62 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2115,32 +2203,32 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2165,37 +2253,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2203,7 +2291,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2228,33 +2316,33 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2262,7 +2350,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2290,52 +2378,52 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2343,27 +2431,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2388,42 +2476,42 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2431,7 +2519,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2459,32 +2547,32 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2492,7 +2580,7 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2519,33 +2607,33 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2553,12 +2641,12 @@
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2569,7 +2657,7 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -2594,18 +2682,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2616,12 +2704,12 @@
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2632,7 +2720,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -2641,81 +2729,66 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
-  <dimension ref="B1:C14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6A5E0-9666-42B8-820C-0803FCEF98B6}">
+  <dimension ref="B1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B15"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
-    <col min="3" max="3" width="109.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>246</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>251</v>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -2726,10 +2799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:B177"/>
+  <dimension ref="B2:B187"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="B187" sqref="B187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2785,7 +2858,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2825,7 +2898,7 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -2985,22 +3058,22 @@
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" s="21" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B63" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
@@ -3015,12 +3088,12 @@
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
@@ -3030,22 +3103,22 @@
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
@@ -3055,32 +3128,32 @@
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="81" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B81" s="19" t="s">
-        <v>120</v>
+        <v>287</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
@@ -3100,7 +3173,7 @@
     </row>
     <row r="86" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B86" s="19" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
@@ -3120,7 +3193,7 @@
     </row>
     <row r="91" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B91" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
@@ -3140,7 +3213,7 @@
     </row>
     <row r="96" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B96" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="97" spans="2:2" x14ac:dyDescent="0.25">
@@ -3155,22 +3228,22 @@
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="100" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B100" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="103" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B103" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
@@ -3185,22 +3258,22 @@
     </row>
     <row r="106" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B106" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="110" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B110" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
@@ -3215,22 +3288,22 @@
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="117" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B117" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
@@ -3250,7 +3323,7 @@
     </row>
     <row r="122" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B122" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
@@ -3270,7 +3343,7 @@
     </row>
     <row r="127" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B127" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
@@ -3290,7 +3363,7 @@
     </row>
     <row r="132" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B132" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="133" spans="2:2" x14ac:dyDescent="0.25">
@@ -3310,7 +3383,7 @@
     </row>
     <row r="137" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B137" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="138" spans="2:2" x14ac:dyDescent="0.25">
@@ -3330,7 +3403,7 @@
     </row>
     <row r="142" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B142" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="143" spans="2:2" x14ac:dyDescent="0.25">
@@ -3345,7 +3418,7 @@
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
@@ -3355,12 +3428,12 @@
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
@@ -3410,7 +3483,7 @@
     </row>
     <row r="158" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B158" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
@@ -3420,17 +3493,17 @@
     </row>
     <row r="161" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B161" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
@@ -3440,27 +3513,27 @@
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="21" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
@@ -3470,37 +3543,82 @@
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="21" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="21" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="18" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B179" s="19" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B180" s="18" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B181" s="18" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B182" s="18" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B183" s="18" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B184" s="18" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B185" s="21" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B186" s="21" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B187" s="18" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3510,66 +3628,81 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6A5E0-9666-42B8-820C-0803FCEF98B6}">
-  <dimension ref="B1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
+  <dimension ref="B1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B1" sqref="B1:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="28" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23"/>
     </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
@@ -3579,13 +3712,154 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{646BF52C-F02F-4980-9FBC-5E2F521BB50A}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F453C7-F3E3-4874-9FCA-AA3F6AA509A3}">
+  <dimension ref="B1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3476811A-3061-4775-AFF8-1D8E59D8890D}">
+  <dimension ref="B1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3595,7 +3869,7 @@
   <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3644,6 +3918,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3706,24 +3981,24 @@
     </row>
     <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>275</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="7" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>277</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="2:8" s="18" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -3876,49 +4151,49 @@
   <sheetData>
     <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
     </row>
     <row r="7" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
@@ -3930,14 +4205,14 @@
     </row>
     <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
     </row>
     <row r="10" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -3949,7 +4224,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -3980,42 +4255,42 @@
   <sheetData>
     <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
     </row>
     <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
     </row>
     <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C5" s="18"/>
       <c r="D5" s="18"/>
     </row>
     <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
@@ -4023,7 +4298,7 @@
     <row r="7" spans="2:4" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18"/>
@@ -4035,7 +4310,7 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
@@ -4075,57 +4350,57 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4138,7 +4413,7 @@
   <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4148,56 +4423,56 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C7" s="24"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C8" s="24"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C9" s="24"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C10" s="24"/>
     </row>
@@ -4206,17 +4481,17 @@
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -4224,7 +4499,7 @@
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-1084: update template and fix issue
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC19309-E6A7-459C-931A-40EF1FFD8E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7620B41-E86B-42FD-99CC-F4C127C3DC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="846" firstSheet="14" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId20"/>
     <sheet name="3-OMGTechDebt" sheetId="30" r:id="rId21"/>
     <sheet name="3-OMGTechDebtDetails" sheetId="31" r:id="rId22"/>
+    <sheet name="3 - Evolution of iso TD" sheetId="32" r:id="rId23"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="312">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1179,6 +1180,101 @@
   <si>
     <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_TABLE</t>
   </si>
+  <si>
+    <t>3.8.	Evolution of OMG Technical Debt</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>MORE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>=true : add this one if you want to get the BC attached to ISO or CISQ with their contributors (if false or not specified you will directly have the contributors for the ID)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>EVOLUTION</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>=true|false to display added and removed technical debt columns. By default or if not exists, is true if there is a previous snapshot.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>HEADER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>=NO to not display headers (useful for excel report when you want to define your own customized headers). By default if option is not present or different from NO, headers are displayed</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>- ID=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">ISO or CISQ </t>
+    </r>
+  </si>
+  <si>
+    <t>Requires installation of OMG Technical Debt Measure (&gt;2.0.0 funcrel) (and ISO-5055 Index extensions and/or CISQ Index extensions).</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_EVOLUTION;ID=ISO,MORE=true,HEADER=NO</t>
+  </si>
 </sst>
 </file>
 
@@ -1187,7 +1283,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1378,6 +1474,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1442,7 +1545,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1524,6 +1627,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1906,7 +2012,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -3864,6 +3970,84 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F19727-0A4D-46F0-B892-29E8A396F1FB}">
+  <dimension ref="B1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="38" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:C6"/>

</xml_diff>

<commit_message>
REPORTGEN-1082: New table application component OMG_TECHNICAL_DEBT_RULES_EVOLUTION
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7620B41-E86B-42FD-99CC-F4C127C3DC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5756E228-475F-40A0-BFAF-DADB04FAFF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="846" firstSheet="14" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -36,6 +36,7 @@
     <sheet name="3-OMGTechDebt" sheetId="30" r:id="rId21"/>
     <sheet name="3-OMGTechDebtDetails" sheetId="31" r:id="rId22"/>
     <sheet name="3 - Evolution of iso TD" sheetId="32" r:id="rId23"/>
+    <sheet name="3 - Rules evolution reg. Omg TD" sheetId="33" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="317">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1274,6 +1275,44 @@
   </si>
   <si>
     <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_EVOLUTION;ID=ISO,MORE=true,HEADER=NO</t>
+  </si>
+  <si>
+    <t>* Block Name = OMG_TECHNICAL_DEBT_EVOLUTION</t>
+  </si>
+  <si>
+    <t>* Block Name = OMG_TECHNICAL_DEBT_RULES_EVOLUTION</t>
+  </si>
+  <si>
+    <r>
+      <t>- ID=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>name of index, like ‘ISO-5055-Security’</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Corbel"/>
+        <family val="2"/>
+      </rPr>
+      <t>DESC=true : add this one if you want to display the rules descriptions (false by default)</t>
+    </r>
+  </si>
+  <si>
+    <t>RepGen:TABLE;OMG_TECHNICAL_DEBT_RULES_EVOLUTION;ID=ISO-5055-Security,DESC=true,HEADER=NO</t>
   </si>
 </sst>
 </file>
@@ -1545,7 +1584,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1613,6 +1652,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
@@ -1628,7 +1670,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2012,7 +2054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2035,8 +2077,8 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D1" s="4"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="6"/>
@@ -2047,16 +2089,16 @@
       <c r="G2" s="14"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
       <c r="D3" s="3"/>
       <c r="E3" s="8"/>
       <c r="F3" s="1"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
       <c r="D4" s="3"/>
       <c r="E4" s="8"/>
       <c r="F4" s="1"/>
@@ -2104,26 +2146,26 @@
       </c>
     </row>
     <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
       <c r="F20" s="10"/>
     </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
       <c r="F21" s="11"/>
-      <c r="G21" s="35"/>
-      <c r="H21" s="35"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="33"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
       <c r="F22" s="11"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
+      <c r="G22" s="36"/>
+      <c r="H22" s="36"/>
     </row>
     <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
@@ -3974,7 +4016,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F19727-0A4D-46F0-B892-29E8A396F1FB}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C80DEE1-1402-4F3F-9664-8981C357215E}">
+  <dimension ref="B1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -3991,55 +4111,50 @@
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>176</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="38" t="s">
-        <v>309</v>
+      <c r="B3" s="33" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
-        <v>306</v>
+      <c r="B4" s="39" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>290</v>
-      </c>
+      <c r="B10" s="25"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="25"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>311</v>
+      <c r="B11" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-1096: User can filter functions with 0 FP in AEFP_LIST component
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{686C4123-D892-46BC-B790-A40B8C5BB5EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3CC738-711E-4938-A689-A778D8A140A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="846" firstSheet="14" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="319">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1316,6 +1316,9 @@
   </si>
   <si>
     <t>* OMG=true : add this option if you have selected an ISO index and want only rules with omg tech debt to be selected (by default it is false). This option has no effect on selection by QR or quality standard tag.</t>
+  </si>
+  <si>
+    <t>ZERO=YES|NO to display the function with 0 AEP (yes by default)</t>
   </si>
 </sst>
 </file>
@@ -2057,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2613,10 +2616,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B587AA6-980F-4560-B177-B792E0F411FE}">
-  <dimension ref="B1:B11"/>
+  <dimension ref="B1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,20 +2664,25 @@
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="18" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23"/>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="22"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3782,7 +3790,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
   <dimension ref="B1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
REPORTGEN-1195: update library templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Temp\RG\Templates\Application\Component library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58523B54-3F57-4D88-B4B9-358076096F9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D625E08-7805-4687-AA18-DF102033EFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5085" yWindow="2085" windowWidth="28800" windowHeight="15345" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="320">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -2062,7 +2062,7 @@
   <dimension ref="B1:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,10 +2197,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
-  <dimension ref="B1:C14"/>
+  <dimension ref="B1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,26 +2250,31 @@
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
+      <c r="B9" s="23" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>173</v>
-      </c>
+      <c r="B10" s="23"/>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-    </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B13" s="23"/>
+    </row>
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>179</v>
       </c>
     </row>
@@ -2757,7 +2762,7 @@
   <dimension ref="B1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4731,10 +4736,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
-  <dimension ref="B1:C16"/>
+  <dimension ref="B1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4798,28 +4803,34 @@
       <c r="C10" s="24"/>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
+      <c r="B11" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="C11" s="24"/>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>173</v>
-      </c>
+      <c r="B12" s="23"/>
     </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>197</v>
       </c>
     </row>

</xml_diff>

<commit_message>
REPORTGEN-1233: add compliance and count options to QUALITY_STANDARDS_EVOLUTION component
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,42 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D625E08-7805-4687-AA18-DF102033EFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D25189-3C8A-4119-82B9-4996C7D8B11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="4680" windowWidth="28800" windowHeight="15345" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
-    <sheet name="2 - Text blocks" sheetId="8" r:id="rId2"/>
-    <sheet name="3 - Table Block - HF" sheetId="10" r:id="rId3"/>
-    <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId4"/>
-    <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
-    <sheet name="3 - List of violations for rule" sheetId="12" r:id="rId6"/>
-    <sheet name="3 - Action Plan Violations" sheetId="13" r:id="rId7"/>
-    <sheet name="3 - Critical Violations List" sheetId="14" r:id="rId8"/>
-    <sheet name="3 - List of violations statist " sheetId="15" r:id="rId9"/>
-    <sheet name="3 - Evolution of standards" sheetId="16" r:id="rId10"/>
-    <sheet name="3 - Top Components" sheetId="18" r:id="rId11"/>
-    <sheet name="3 - Rules with largest variatio" sheetId="19" r:id="rId12"/>
-    <sheet name="3 - Removed violations" sheetId="20" r:id="rId13"/>
-    <sheet name="3 - components by status list" sheetId="22" r:id="rId14"/>
-    <sheet name="3 - AEFP list" sheetId="23" r:id="rId15"/>
-    <sheet name="3 - AETP list" sheetId="24" r:id="rId16"/>
-    <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId17"/>
-    <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId18"/>
-    <sheet name="3-ActionPlanBookmarksTable" sheetId="28" r:id="rId19"/>
-    <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId20"/>
-    <sheet name="3-OMGTechDebt" sheetId="30" r:id="rId21"/>
-    <sheet name="3-OMGTechDebtDetails" sheetId="31" r:id="rId22"/>
-    <sheet name="3 - Evolution of iso TD" sheetId="32" r:id="rId23"/>
-    <sheet name="3 - Rules evolution reg. Omg TD" sheetId="33" r:id="rId24"/>
+    <sheet name="Sheet1" sheetId="34" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="35" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="36" r:id="rId4"/>
+    <sheet name="2 - Text blocks" sheetId="8" r:id="rId5"/>
+    <sheet name="3 - Table Block - HF" sheetId="10" r:id="rId6"/>
+    <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId7"/>
+    <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId8"/>
+    <sheet name="3 - List of violations for rule" sheetId="12" r:id="rId9"/>
+    <sheet name="3 - Action Plan Violations" sheetId="13" r:id="rId10"/>
+    <sheet name="3 - Critical Violations List" sheetId="14" r:id="rId11"/>
+    <sheet name="3 - List of violations statist " sheetId="15" r:id="rId12"/>
+    <sheet name="3 - Evolution of standards" sheetId="16" r:id="rId13"/>
+    <sheet name="3 - Top Components" sheetId="18" r:id="rId14"/>
+    <sheet name="3 - Rules with largest variatio" sheetId="19" r:id="rId15"/>
+    <sheet name="3 - Removed violations" sheetId="20" r:id="rId16"/>
+    <sheet name="3 - components by status list" sheetId="22" r:id="rId17"/>
+    <sheet name="3 - AEFP list" sheetId="23" r:id="rId18"/>
+    <sheet name="3 - AETP list" sheetId="24" r:id="rId19"/>
+    <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId20"/>
+    <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId21"/>
+    <sheet name="3-ActionPlanBookmarksTable" sheetId="28" r:id="rId22"/>
+    <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId23"/>
+    <sheet name="3-OMGTechDebt" sheetId="30" r:id="rId24"/>
+    <sheet name="3-OMGTechDebtDetails" sheetId="31" r:id="rId25"/>
+    <sheet name="3 - Evolution of iso TD" sheetId="32" r:id="rId26"/>
+    <sheet name="3 - Rules evolution reg. Omg TD" sheetId="33" r:id="rId27"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -62,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="322">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -597,9 +600,6 @@
   </si>
   <si>
     <t>* STD= Name of the parent quality standard you want the details, for example, CWE-2011-Top25 will list total, added and removed violations for standards CWE-22, CWE-78, CWE-79, CWE-89, CWE-134, CWE-327, CWE-434 and CWE-798.</t>
-  </si>
-  <si>
-    <t>To use this component, the Quality Standards Mapping extension should be installed on the central where the application resides, with minimum version 20181030</t>
   </si>
   <si>
     <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=CWE-2011-Top25</t>
@@ -1322,6 +1322,15 @@
   </si>
   <si>
     <t>To use this component, the following extensions should be installed : Quality standards mapping extension &gt;= 20240212.0.0-funcrel;CISQ index extension &gt;= 20240201.0.0-funcrel;ISO-5055 index extension &gt;= 20240202;Security Standards extension &gt;= 20240209.0.0-funcrel</t>
+  </si>
+  <si>
+    <t>To use this component, the Quality Standards Mapping extension, or an extensions managing quality index should be installed on the central where the application resides, with minimum version 20181030</t>
+  </si>
+  <si>
+    <t>* COMPLIANCE=true|false(false per default) to display the compliance score in percent for the current BC/TC. Not applicable for a quality standard</t>
+  </si>
+  <si>
+    <t>* COUNT= the number of rows to display (all rows when nothing specified, or -1)</t>
   </si>
 </sst>
 </file>
@@ -2062,7 +2071,7 @@
   <dimension ref="B1:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2196,11 +2205,179 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
-  <dimension ref="B1:C15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F8858A-750A-4726-A1F9-D59D03327DAC}">
+  <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+    </row>
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="2:4" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F955B29-1E36-48CE-AC50-446125F25D1B}">
+  <dimension ref="B1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
+  <dimension ref="B1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,72 +2387,89 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>225</v>
+        <v>168</v>
       </c>
       <c r="C1" s="29"/>
     </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>177</v>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
-        <v>264</v>
+      <c r="B4" s="23" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>226</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>227</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>250</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="C7" s="24"/>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>251</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>318</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="C9" s="24"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
+      <c r="B10" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="24"/>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-    </row>
     <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>179</v>
+      <c r="B14" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -2284,7 +2478,106 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
+  <dimension ref="B1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="23"/>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A48014B-133C-4EB1-BCC8-C47F0FE2BA42}">
   <dimension ref="B1:B20"/>
   <sheetViews>
@@ -2300,62 +2593,62 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2363,32 +2656,32 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="27" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="2:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="30" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="2:2" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="30" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2397,7 +2690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321A33B9-4108-40C7-AB52-19B5A9656C7B}">
   <dimension ref="B1:B10"/>
   <sheetViews>
@@ -2413,37 +2706,37 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2451,7 +2744,7 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2460,7 +2753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53E83-8DB2-4C9D-B684-50883B392432}">
   <dimension ref="B1:I9"/>
   <sheetViews>
@@ -2476,33 +2769,33 @@
   <sheetData>
     <row r="1" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I1" s="26"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2510,7 +2803,7 @@
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2522,7 +2815,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6911279-FAB1-4631-AA51-7D78BAFCA198}">
   <dimension ref="B1:B17"/>
   <sheetViews>
@@ -2538,52 +2831,52 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
@@ -2591,27 +2884,27 @@
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="25" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="25" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2620,7 +2913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B587AA6-980F-4560-B177-B792E0F411FE}">
   <dimension ref="B1:B12"/>
   <sheetViews>
@@ -2636,42 +2929,42 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
@@ -2684,7 +2977,7 @@
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2696,7 +2989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822C81FE-2BA1-4A3C-ADB8-F42B4B1305BA}">
   <dimension ref="B1:B9"/>
   <sheetViews>
@@ -2712,27 +3005,27 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
@@ -2745,7 +3038,7 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2757,7 +3050,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8781DFF-DE06-4E2B-B3D7-80F693AF2C98}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
   <dimension ref="B1:C13"/>
   <sheetViews>
@@ -2772,38 +3077,38 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2816,7 +3121,7 @@
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2827,7 +3132,7 @@
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2836,7 +3141,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A93F7-09DE-4CB9-9DC0-106F29CE8F69}">
   <dimension ref="B1:C10"/>
   <sheetViews>
@@ -2852,18 +3157,18 @@
   <sheetData>
     <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B1" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C1" s="29"/>
     </row>
     <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2879,7 +3184,7 @@
     </row>
     <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -2890,7 +3195,7 @@
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2898,7 +3203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6A5E0-9666-42B8-820C-0803FCEF98B6}">
   <dimension ref="B1:B12"/>
   <sheetViews>
@@ -2910,32 +3215,32 @@
   <sheetData>
     <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="19" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B2" s="28" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="28" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2948,17 +3253,17 @@
     </row>
     <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="23" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -2967,7 +3272,424 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
+  <dimension ref="B1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F453C7-F3E3-4874-9FCA-AA3F6AA509A3}">
+  <dimension ref="B1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3476811A-3061-4775-AFF8-1D8E59D8890D}">
+  <dimension ref="B1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F19727-0A4D-46F0-B892-29E8A396F1FB}">
+  <dimension ref="B1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C80DEE1-1402-4F3F-9664-8981C357215E}">
+  <dimension ref="B1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9DE975-16AA-4717-A977-51023EE1E71B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BA0B77-88B8-4878-A421-8FC44413067F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B187"/>
   <sheetViews>
@@ -3278,17 +4000,17 @@
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
@@ -3298,32 +4020,32 @@
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="18" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="81" spans="2:2" s="19" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B81" s="19" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
@@ -3588,7 +4310,7 @@
     </row>
     <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="146" spans="2:2" x14ac:dyDescent="0.25">
@@ -3598,12 +4320,12 @@
     </row>
     <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="149" spans="2:2" x14ac:dyDescent="0.25">
@@ -3653,7 +4375,7 @@
     </row>
     <row r="158" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B158" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="159" spans="2:2" x14ac:dyDescent="0.25">
@@ -3663,17 +4385,17 @@
     </row>
     <row r="161" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B161" s="19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="162" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B162" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="163" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B163" s="18" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="164" spans="2:2" x14ac:dyDescent="0.25">
@@ -3683,27 +4405,27 @@
     </row>
     <row r="165" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B165" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="166" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B166" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="167" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B167" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="168" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B168" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="169" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B169" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="170" spans="2:2" x14ac:dyDescent="0.25">
@@ -3713,82 +4435,82 @@
     </row>
     <row r="171" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B171" s="21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="172" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B172" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="173" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B173" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="174" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B174" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="175" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B175" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="176" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B176" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="177" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B177" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="179" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B179" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="180" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B180" s="18" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="181" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B181" s="18" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="182" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B182" s="18" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="183" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B183" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="184" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B184" s="18" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="185" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B185" s="21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="186" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B186" s="21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -3797,400 +4519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
-  <dimension ref="B1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
-    <col min="3" max="3" width="109.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>244</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>249</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F453C7-F3E3-4874-9FCA-AA3F6AA509A3}">
-  <dimension ref="B1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="40.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>303</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3476811A-3061-4775-AFF8-1D8E59D8890D}">
-  <dimension ref="B1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="40.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F19727-0A4D-46F0-B892-29E8A396F1FB}">
-  <dimension ref="B1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="25"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>310</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C80DEE1-1402-4F3F-9664-8981C357215E}">
-  <dimension ref="B1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>304</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="25"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>315</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:C6"/>
   <sheetViews>
@@ -4248,7 +4577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H12"/>
   <sheetViews>
@@ -4307,18 +4636,18 @@
     </row>
     <row r="6" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>273</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="7" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
+        <v>274</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>275</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="8" spans="2:8" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4348,7 +4677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
@@ -4462,7 +4791,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:D13"/>
   <sheetViews>
@@ -4564,278 +4893,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F8858A-750A-4726-A1F9-D59D03327DAC}">
-  <dimension ref="B1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-    </row>
-    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-    </row>
-    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-    </row>
-    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>282</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-    </row>
-    <row r="7" spans="2:4" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F955B29-1E36-48CE-AC50-446125F25D1B}">
-  <dimension ref="B1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
-  <dimension ref="B1:C17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>226</v>
-      </c>
-      <c r="C7" s="24"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>242</v>
-      </c>
-      <c r="C9" s="24"/>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>251</v>
-      </c>
-      <c r="C10" s="24"/>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>318</v>
-      </c>
-      <c r="C11" s="24"/>
-    </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>197</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
REPORTGEN-1235: add count to limit the number of rows in QUALITY_STANDARDS_EVOLUTION and QUALITY_TAGS_RULES_EVOLUTION components
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D25189-3C8A-4119-82B9-4996C7D8B11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CACEEDB-0111-4326-B127-B357DDF55920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="846" firstSheet="9" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="322">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -2070,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -2483,7 +2483,7 @@
   <dimension ref="B1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3064,10 +3064,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
-  <dimension ref="B1:C13"/>
+  <dimension ref="B1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3112,26 +3112,31 @@
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
+      <c r="B8" s="23" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>173</v>
-      </c>
+      <c r="B9" s="23"/>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-    </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>228</v>
       </c>
     </row>

</xml_diff>

<commit_message>
REPORTGEN-1234: add compliance to QUALITY_TAGS_RULES_EVOLUTION component
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,38 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CACEEDB-0111-4326-B127-B357DDF55920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EF9BA0-F252-4D75-8D4D-5D32982C9972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="846" firstSheet="9" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="34" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="35" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="36" r:id="rId4"/>
-    <sheet name="2 - Text blocks" sheetId="8" r:id="rId5"/>
-    <sheet name="3 - Table Block - HF" sheetId="10" r:id="rId6"/>
-    <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId7"/>
-    <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId8"/>
-    <sheet name="3 - List of violations for rule" sheetId="12" r:id="rId9"/>
-    <sheet name="3 - Action Plan Violations" sheetId="13" r:id="rId10"/>
-    <sheet name="3 - Critical Violations List" sheetId="14" r:id="rId11"/>
-    <sheet name="3 - List of violations statist " sheetId="15" r:id="rId12"/>
-    <sheet name="3 - Evolution of standards" sheetId="16" r:id="rId13"/>
-    <sheet name="3 - Top Components" sheetId="18" r:id="rId14"/>
-    <sheet name="3 - Rules with largest variatio" sheetId="19" r:id="rId15"/>
-    <sheet name="3 - Removed violations" sheetId="20" r:id="rId16"/>
-    <sheet name="3 - components by status list" sheetId="22" r:id="rId17"/>
-    <sheet name="3 - AEFP list" sheetId="23" r:id="rId18"/>
-    <sheet name="3 - AETP list" sheetId="24" r:id="rId19"/>
-    <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId20"/>
-    <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId21"/>
-    <sheet name="3-ActionPlanBookmarksTable" sheetId="28" r:id="rId22"/>
-    <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId23"/>
-    <sheet name="3-OMGTechDebt" sheetId="30" r:id="rId24"/>
-    <sheet name="3-OMGTechDebtDetails" sheetId="31" r:id="rId25"/>
-    <sheet name="3 - Evolution of iso TD" sheetId="32" r:id="rId26"/>
-    <sheet name="3 - Rules evolution reg. Omg TD" sheetId="33" r:id="rId27"/>
+    <sheet name="2 - Text blocks" sheetId="8" r:id="rId2"/>
+    <sheet name="3 - Table Block - HF" sheetId="10" r:id="rId3"/>
+    <sheet name="3 - Table Block - AFP" sheetId="9" r:id="rId4"/>
+    <sheet name="3 - Table Block - Violations" sheetId="11" r:id="rId5"/>
+    <sheet name="3 - List of violations for rule" sheetId="12" r:id="rId6"/>
+    <sheet name="3 - Action Plan Violations" sheetId="13" r:id="rId7"/>
+    <sheet name="3 - Critical Violations List" sheetId="14" r:id="rId8"/>
+    <sheet name="3 - List of violations statist " sheetId="15" r:id="rId9"/>
+    <sheet name="3 - Evolution of standards" sheetId="16" r:id="rId10"/>
+    <sheet name="3 - Top Components" sheetId="18" r:id="rId11"/>
+    <sheet name="3 - Rules with largest variatio" sheetId="19" r:id="rId12"/>
+    <sheet name="3 - Removed violations" sheetId="20" r:id="rId13"/>
+    <sheet name="3 - components by status list" sheetId="22" r:id="rId14"/>
+    <sheet name="3 - AEFP list" sheetId="23" r:id="rId15"/>
+    <sheet name="3 - AETP list" sheetId="24" r:id="rId16"/>
+    <sheet name="3-CastRulesEvoByQualityCategory" sheetId="25" r:id="rId17"/>
+    <sheet name="3-ListTagsDocByCat" sheetId="26" r:id="rId18"/>
+    <sheet name="3-ActionPlanBookmarksTable" sheetId="28" r:id="rId19"/>
+    <sheet name="3-ListViolBookmarks" sheetId="27" r:id="rId20"/>
+    <sheet name="3-OMGTechDebt" sheetId="30" r:id="rId21"/>
+    <sheet name="3-OMGTechDebtDetails" sheetId="31" r:id="rId22"/>
+    <sheet name="3 - Evolution of iso TD" sheetId="32" r:id="rId23"/>
+    <sheet name="3 - Rules evolution reg. Omg TD" sheetId="33" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">'1 - Information'!$C$20:$F$23</definedName>
@@ -65,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="323">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1331,6 +1328,9 @@
   </si>
   <si>
     <t>* COUNT= the number of rows to display (all rows when nothing specified, or -1)</t>
+  </si>
+  <si>
+    <t>* COMPLIANCE=true|false(false per default) to display the compliance score in percent for the current BC/TC/QR. Not applicable for a quality standard</t>
   </si>
 </sst>
 </file>
@@ -2070,7 +2070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O23"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -2205,285 +2205,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F8858A-750A-4726-A1F9-D59D03327DAC}">
-  <dimension ref="B1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="54.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-    </row>
-    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="23" t="s">
-        <v>149</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-    </row>
-    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-    </row>
-    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>281</v>
-      </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-    </row>
-    <row r="7" spans="2:4" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-    </row>
-    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>151</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F955B29-1E36-48CE-AC50-446125F25D1B}">
-  <dimension ref="B1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
-  <dimension ref="B1:C17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>225</v>
-      </c>
-      <c r="C7" s="24"/>
-    </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>240</v>
-      </c>
-      <c r="C8" s="24"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>241</v>
-      </c>
-      <c r="C9" s="24"/>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>250</v>
-      </c>
-      <c r="C10" s="24"/>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>317</v>
-      </c>
-      <c r="C11" s="24"/>
-    </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
   <dimension ref="B1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,7 +2303,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A48014B-133C-4EB1-BCC8-C47F0FE2BA42}">
   <dimension ref="B1:B20"/>
   <sheetViews>
@@ -2690,7 +2416,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321A33B9-4108-40C7-AB52-19B5A9656C7B}">
   <dimension ref="B1:B10"/>
   <sheetViews>
@@ -2753,7 +2479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9C53E83-8DB2-4C9D-B684-50883B392432}">
   <dimension ref="B1:I9"/>
   <sheetViews>
@@ -2815,7 +2541,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6911279-FAB1-4631-AA51-7D78BAFCA198}">
   <dimension ref="B1:B17"/>
   <sheetViews>
@@ -2913,7 +2639,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B587AA6-980F-4560-B177-B792E0F411FE}">
   <dimension ref="B1:B12"/>
   <sheetViews>
@@ -2989,7 +2715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{822C81FE-2BA1-4A3C-ADB8-F42B4B1305BA}">
   <dimension ref="B1:B9"/>
   <sheetViews>
@@ -3050,24 +2776,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8781DFF-DE06-4E2B-B3D7-80F693AF2C98}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
+  <dimension ref="B1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
-  <dimension ref="B1:C14"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,26 +2831,31 @@
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
+      <c r="B9" s="23" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>173</v>
-      </c>
+      <c r="B10" s="23"/>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-    </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-    </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B13" s="23"/>
+    </row>
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>228</v>
       </c>
     </row>
@@ -3146,7 +2865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8A93F7-09DE-4CB9-9DC0-106F29CE8F69}">
   <dimension ref="B1:C10"/>
   <sheetViews>
@@ -3208,7 +2927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A6A5E0-9666-42B8-820C-0803FCEF98B6}">
   <dimension ref="B1:B12"/>
   <sheetViews>
@@ -3277,424 +2996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
-  <dimension ref="B1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="90.28515625" customWidth="1"/>
-    <col min="3" max="3" width="109.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>243</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-    </row>
-    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>248</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F453C7-F3E3-4874-9FCA-AA3F6AA509A3}">
-  <dimension ref="B1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="40.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="32" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>302</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3476811A-3061-4775-AFF8-1D8E59D8890D}">
-  <dimension ref="B1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="40.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B1" s="19" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="31" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-    </row>
-    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>299</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F19727-0A4D-46F0-B892-29E8A396F1FB}">
-  <dimension ref="B1:C12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="25" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="25"/>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>309</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C80DEE1-1402-4F3F-9664-8981C357215E}">
-  <dimension ref="B1:C11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="B1" s="19" t="s">
-        <v>303</v>
-      </c>
-      <c r="C1" s="29"/>
-    </row>
-    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="33" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="25" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="25" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="25"/>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>314</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE9DE975-16AA-4717-A977-51023EE1E71B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BA0B77-88B8-4878-A421-8FC44413067F}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:B187"/>
   <sheetViews>
@@ -4524,7 +3826,400 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A3C08B-030D-4CD0-9D7A-3D29C37EEAE3}">
+  <dimension ref="B1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="90.28515625" customWidth="1"/>
+    <col min="3" max="3" width="109.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>248</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53F453C7-F3E3-4874-9FCA-AA3F6AA509A3}">
+  <dimension ref="B1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3476811A-3061-4775-AFF8-1D8E59D8890D}">
+  <dimension ref="B1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="40.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="28" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="31" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>299</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F19727-0A4D-46F0-B892-29E8A396F1FB}">
+  <dimension ref="B1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="25"/>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>309</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C80DEE1-1402-4F3F-9664-8981C357215E}">
+  <dimension ref="B1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="28" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="33" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="34" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="24" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="25" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="25"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:C6"/>
   <sheetViews>
@@ -4582,7 +4277,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:H12"/>
   <sheetViews>
@@ -4682,7 +4377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:C14"/>
   <sheetViews>
@@ -4796,7 +4491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:D13"/>
   <sheetViews>
@@ -4898,4 +4593,278 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F8858A-750A-4726-A1F9-D59D03327DAC}">
+  <dimension ref="B1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+    </row>
+    <row r="3" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B3" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+    </row>
+    <row r="6" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="2:4" s="22" customFormat="1" ht="15.75" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+    </row>
+    <row r="9" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="22"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F955B29-1E36-48CE-AC50-446125F25D1B}">
+  <dimension ref="B1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="92.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B1" s="19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>155</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{976C8EF6-9462-404B-9CE3-9B69F0A9930C}">
+  <dimension ref="B1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="121.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="21" x14ac:dyDescent="0.35">
+      <c r="B1" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="29"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" s="24"/>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="23" t="s">
+        <v>240</v>
+      </c>
+      <c r="C8" s="24"/>
+    </row>
+    <row r="9" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="23" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="24"/>
+    </row>
+    <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="23" t="s">
+        <v>250</v>
+      </c>
+      <c r="C10" s="24"/>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="C11" s="24"/>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
REPORTGEN-1236: implement new component TOTAL_VIOLATIONS
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EF9BA0-F252-4D75-8D4D-5D32982C9972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AF94F7-0781-4820-ADDF-73FBEB0BB84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="328">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1331,6 +1331,21 @@
   </si>
   <si>
     <t>* COMPLIANCE=true|false(false per default) to display the compliance score in percent for the current BC/TC/QR. Not applicable for a quality standard</t>
+  </si>
+  <si>
+    <t>2.28. -nb of total violations per metric</t>
+  </si>
+  <si>
+    <t>* Block Name =TOTAL_VIOLATIONS</t>
+  </si>
+  <si>
+    <t>- ID=BC id, or TC id, or quality rule id</t>
+  </si>
+  <si>
+    <t>- CRITICAL=true|false to get the number of critical violations only (false by default)</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;TOTAL_VIOLATIONS;ID=60017</t>
   </si>
 </sst>
 </file>
@@ -2998,10 +3013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:B187"/>
+  <dimension ref="B2:B195"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B187" sqref="B187"/>
+    <sheetView topLeftCell="A165" workbookViewId="0">
+      <selection activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3818,6 +3833,41 @@
     <row r="187" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B187" s="18" t="s">
         <v>290</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B189" s="19" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B190" s="18" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B191" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B192" s="21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B193" s="21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B194" s="21" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B195" s="18" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-1237: add component TOTAL_VIOLATIONS_EVOLUTION
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0AF94F7-0781-4820-ADDF-73FBEB0BB84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4E2B1F-0DBC-4770-9B13-3AD024C85C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="332">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1346,6 +1346,18 @@
   </si>
   <si>
     <t>RepGen:TEXT;TOTAL_VIOLATIONS;ID=60017</t>
+  </si>
+  <si>
+    <t>2.29. -Evolution of the nb of total violations per metric</t>
+  </si>
+  <si>
+    <t>* Block Name =TOTAL_VIOLATIONS_EVOLUTION</t>
+  </si>
+  <si>
+    <t>- FORMAT=PERCENT (number by default)</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;TOTAL_VIOLATIONS_EVOLUTION;ID=60017</t>
   </si>
 </sst>
 </file>
@@ -3013,10 +3025,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:B195"/>
+  <dimension ref="B2:B204"/>
   <sheetViews>
     <sheetView topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="B196" sqref="B196"/>
+      <selection activeCell="B206" sqref="B206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3868,6 +3880,41 @@
     <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" s="18" t="s">
         <v>327</v>
+      </c>
+    </row>
+    <row r="198" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B198" s="19" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B199" s="18" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B200" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B201" s="21" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B202" s="21" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B203" s="21" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B204" s="18" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-1239: feedback on quality_tag_rule_evolution
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29725"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4E2B1F-0DBC-4770-9B13-3AD024C85C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE89F69-D3CF-4A56-B937-866DFAA62ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28695" yWindow="10320" windowWidth="28800" windowHeight="15345" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="333">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1358,6 +1358,9 @@
   </si>
   <si>
     <t>RepGen:TEXT;TOTAL_VIOLATIONS_EVOLUTION;ID=60017</t>
+  </si>
+  <si>
+    <t>* EVOLUTION=true|false to display added and removed violations columns. By default or if not exists, is true</t>
   </si>
 </sst>
 </file>
@@ -2098,7 +2101,7 @@
   <dimension ref="B1:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2805,10 +2808,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
-  <dimension ref="B1:C15"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,26 +2866,31 @@
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
+      <c r="B10" s="23" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>173</v>
-      </c>
+      <c r="B11" s="23"/>
     </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="23" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-    </row>
     <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="22"/>
-    </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B14" s="23"/>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="22"/>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>228</v>
       </c>
     </row>

</xml_diff>

<commit_message>
REPORTGEN-1239: implement feedbacks for ISO-5055
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Component library/3- Excel-components-library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Component library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE89F69-D3CF-4A56-B937-866DFAA62ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8228138B-D817-4ED9-8647-2C0CC248363E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28695" yWindow="10320" windowWidth="28800" windowHeight="15345" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15345" tabRatio="846" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1 - Information" sheetId="6" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="334">
   <si>
     <t>RepGen:TEXT;APPLICATION_NAME</t>
   </si>
@@ -1361,6 +1361,9 @@
   </si>
   <si>
     <t>* EVOLUTION=true|false to display added and removed violations columns. By default or if not exists, is true</t>
+  </si>
+  <si>
+    <t>* SORTBYCOMPLIANCE=asc|desc|false (false per default), if present will sort the current table by compliance score asc or desc</t>
   </si>
 </sst>
 </file>
@@ -2101,7 +2104,7 @@
   <dimension ref="B1:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C22" sqref="C22:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2236,10 +2239,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92753F2C-AEBD-49B1-A0DF-FB40FC05FDC6}">
-  <dimension ref="B1:C17"/>
+  <dimension ref="B1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2300,30 +2303,35 @@
     </row>
     <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-    </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
-        <v>173</v>
-      </c>
+      <c r="B13" s="23"/>
     </row>
     <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="23" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-    </row>
     <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B16" s="23"/>
+    </row>
+    <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="22"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2808,7 +2816,7 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88ECF1C8-5AB3-4063-B1EA-9D9688F82C45}">
-  <dimension ref="B1:C16"/>
+  <dimension ref="B1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -2867,30 +2875,35 @@
     </row>
     <row r="10" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="23" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-    </row>
     <row r="12" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>173</v>
-      </c>
+      <c r="B12" s="23"/>
     </row>
     <row r="13" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="23" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-    </row>
     <row r="15" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B15" s="23"/>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="22"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>228</v>
       </c>
     </row>

</xml_diff>